<commit_message>
Fixed some Copy/Paste Errors
</commit_message>
<xml_diff>
--- a/input_data/project_expenses.xlsx
+++ b/input_data/project_expenses.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10613"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10709"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/imhiro/AllFiles/0021_travel_events_conferences_workshops/2018-07-24_europython_edinburgh/notebook/input_data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/imhiro/Desktop/europython2018_boring/input_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A05E6084-0C7C-2C44-B09D-B3449B2ED4F2}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE30CA2E-FC10-FD4B-9BC7-95A9D80568A0}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5560" yWindow="3560" windowWidth="28040" windowHeight="17440" xr2:uid="{142A1978-244E-F549-9C54-5C6C90F4E4C1}"/>
   </bookViews>
@@ -45,9 +45,6 @@
     <t>Dieter</t>
   </si>
   <si>
-    <t>Amount</t>
-  </si>
-  <si>
     <t>Mars Colony</t>
   </si>
   <si>
@@ -88,6 +85,9 @@
   </si>
   <si>
     <t>Description</t>
+  </si>
+  <si>
+    <t>Cost</t>
   </si>
 </sst>
 </file>
@@ -451,7 +451,7 @@
   <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F26" sqref="F26"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -469,10 +469,10 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>20</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -480,10 +480,10 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D2" s="2">
         <v>80</v>
@@ -494,10 +494,10 @@
         <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D3" s="2">
         <v>10</v>
@@ -508,10 +508,10 @@
         <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D4" s="2">
         <v>1000</v>
@@ -522,10 +522,10 @@
         <v>5</v>
       </c>
       <c r="B5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D5" s="2">
         <v>30</v>
@@ -536,10 +536,10 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D6" s="2">
         <v>15</v>
@@ -550,10 +550,10 @@
         <v>2</v>
       </c>
       <c r="B7" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C7" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D7" s="2">
         <v>2</v>
@@ -564,10 +564,10 @@
         <v>2</v>
       </c>
       <c r="B8" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C8" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D8" s="2">
         <v>5</v>
@@ -578,10 +578,10 @@
         <v>4</v>
       </c>
       <c r="B9" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C9" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D9" s="2">
         <v>20</v>
@@ -592,10 +592,10 @@
         <v>4</v>
       </c>
       <c r="B10" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C10" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D10" s="2">
         <v>500</v>
@@ -606,10 +606,10 @@
         <v>5</v>
       </c>
       <c r="B11" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C11" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D11" s="2">
         <v>2.5</v>
@@ -620,10 +620,10 @@
         <v>3</v>
       </c>
       <c r="B12" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C12" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D12" s="2">
         <v>5</v>

</xml_diff>